<commit_message>
email body will go as plaintext
</commit_message>
<xml_diff>
--- a/pythonmailerv1.6/rcvr_mail_list.xlsx
+++ b/pythonmailerv1.6/rcvr_mail_list.xlsx
@@ -48,7 +48,7 @@
     <t xml:space="preserve">NORTON1A2B3C4D5E6F7G8H9I</t>
   </si>
   <si>
-    <t xml:space="preserve">mahidulmoon@gmail.com</t>
+    <t xml:space="preserve">Sarrajusantosh@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -58,7 +58,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,6 +95,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,7 +148,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -156,6 +162,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -237,10 +247,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -280,7 +290,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -293,10 +303,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="dev.abdullah.mamun@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="mahidulmoon@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="Sarrajusantosh@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>